<commit_message>
Wordepress changes, i will start working on new things post this commit
</commit_message>
<xml_diff>
--- a/TestData/DataSet1.xlsx
+++ b/TestData/DataSet1.xlsx
@@ -8,13 +8,14 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
   <si>
     <t>Suraj</t>
   </si>
@@ -50,6 +51,27 @@
   </si>
   <si>
     <t>Rohit</t>
+  </si>
+  <si>
+    <t>raju</t>
+  </si>
+  <si>
+    <t>SSS</t>
+  </si>
+  <si>
+    <t>aazz</t>
+  </si>
+  <si>
+    <t>bb</t>
+  </si>
+  <si>
+    <t>cc</t>
+  </si>
+  <si>
+    <t>dd</t>
+  </si>
+  <si>
+    <t>ee</t>
   </si>
 </sst>
 </file>
@@ -391,10 +413,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -443,6 +465,102 @@
         <v>9</v>
       </c>
     </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>